<commit_message>
I have added a text to interpret my data. This is the final version
</commit_message>
<xml_diff>
--- a/ExcelLab.xlsx
+++ b/ExcelLab.xlsx
@@ -125,8 +125,353 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Arial"/>
+              </a:rPr>
+              <a:t>Average salaries of the jobs that are in most demand in Canada</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$4</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+          </c:spPr>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$5:$B$12</c:f>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$5:$C$12</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="1467516865"/>
+        <c:axId val="1700078498"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1467516865"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t/>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:spPr/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1700078498"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1700078498"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="B7B7B7"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="CCCCCC">
+                  <a:alpha val="0"/>
+                </a:srgbClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t/>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1467516865"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0">
+            <a:defRPr b="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Arial"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+</c:chartSpace>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>514350</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="5715000" cy="3533775"/>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="1" name="Chart 1" title="Chart"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>923925</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="3133725" cy="1828800"/>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Shape 3"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="480325" y="921450"/>
+          <a:ext cx="3117300" cy="1813500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="4A86E8"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr anchorCtr="0" anchor="t" bIns="91425" lIns="91425" spcFirstLastPara="1" rIns="91425" wrap="square" tIns="91425">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr indent="0" lvl="0" marL="0" rtl="0" algn="l">
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buNone/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400">
+              <a:latin typeface="Times New Roman"/>
+              <a:ea typeface="Times New Roman"/>
+              <a:cs typeface="Times New Roman"/>
+              <a:sym typeface="Times New Roman"/>
+            </a:rPr>
+            <a:t>The data represented in this chart refers to the average salaries of the jobs that are the highest in demand in the IT field in Canada. Out of these jobs, “Senior Software Engineer” gets payed the most </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400">
+              <a:latin typeface="Times New Roman"/>
+              <a:ea typeface="Times New Roman"/>
+              <a:cs typeface="Times New Roman"/>
+              <a:sym typeface="Times New Roman"/>
+            </a:rPr>
+            <a:t>(on average)</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400">
+              <a:latin typeface="Times New Roman"/>
+              <a:ea typeface="Times New Roman"/>
+              <a:cs typeface="Times New Roman"/>
+              <a:sym typeface="Times New Roman"/>
+            </a:rPr>
+            <a:t> and Technical Support Specialists get payes the least </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400">
+              <a:latin typeface="Times New Roman"/>
+              <a:ea typeface="Times New Roman"/>
+              <a:cs typeface="Times New Roman"/>
+              <a:sym typeface="Times New Roman"/>
+            </a:rPr>
+            <a:t>(on average)</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400">
+              <a:latin typeface="Times New Roman"/>
+              <a:ea typeface="Times New Roman"/>
+              <a:cs typeface="Times New Roman"/>
+              <a:sym typeface="Times New Roman"/>
+            </a:rPr>
+            <a:t>. </a:t>
+          </a:r>
+          <a:endParaRPr sz="1400">
+            <a:latin typeface="Times New Roman"/>
+            <a:ea typeface="Times New Roman"/>
+            <a:cs typeface="Times New Roman"/>
+            <a:sym typeface="Times New Roman"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>